<commit_message>
otimizando o tempo do original
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -24,9 +24,6 @@
     <t>Original</t>
   </si>
   <si>
-    <t>Hibrido</t>
-  </si>
-  <si>
     <t>RM698_L60</t>
   </si>
   <si>
@@ -54,10 +51,13 @@
     <t>Tempo</t>
   </si>
   <si>
-    <t>NSGA-II</t>
-  </si>
-  <si>
-    <t>Intel (R) Core (TM) i7-6500U CPU @ 2.50GHz</t>
+    <t>Intel (R) Core (TM) i7-6500U CPU @ 2.5GHz 8GB RAM</t>
+  </si>
+  <si>
+    <t>NSGA-II 1</t>
+  </si>
+  <si>
+    <t>NSGA-II Imprv</t>
   </si>
 </sst>
 </file>
@@ -118,11 +118,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -421,188 +421,252 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A5:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.125" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" customWidth="1"/>
+    <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.125" customWidth="1"/>
+    <col min="6" max="6" width="12.375" customWidth="1"/>
+    <col min="7" max="7" width="13.875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>201</v>
+      </c>
+      <c r="C8" s="1">
+        <v>10.87</v>
+      </c>
+      <c r="D8" s="1">
+        <v>210</v>
+      </c>
+      <c r="E8" s="1">
+        <v>25.74</v>
+      </c>
+      <c r="F8" s="1">
+        <v>215</v>
+      </c>
+      <c r="G8" s="1">
+        <v>23.35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2">
-        <v>210</v>
-      </c>
-      <c r="E8" s="2">
-        <v>118.78</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="1">
+        <v>321</v>
+      </c>
+      <c r="C9" s="1">
+        <v>77.180000000000007</v>
+      </c>
+      <c r="D9" s="1">
+        <v>339</v>
+      </c>
+      <c r="E9" s="1">
+        <v>268.88</v>
+      </c>
+      <c r="F9" s="1">
+        <v>348</v>
+      </c>
+      <c r="G9" s="1">
+        <v>249.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2">
-        <v>339</v>
-      </c>
-      <c r="E9" s="2">
-        <v>474.08</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="1">
+        <v>129</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5.97</v>
+      </c>
+      <c r="D10" s="1">
+        <v>135</v>
+      </c>
+      <c r="E10" s="1">
+        <v>9.18</v>
+      </c>
+      <c r="F10" s="1">
+        <v>135</v>
+      </c>
+      <c r="G10" s="1">
+        <v>7.89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2">
-        <v>135</v>
-      </c>
-      <c r="E10" s="2">
-        <v>22.34</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="1">
+        <v>191</v>
+      </c>
+      <c r="C11" s="1">
+        <v>54.7</v>
+      </c>
+      <c r="D11" s="1">
+        <v>205</v>
+      </c>
+      <c r="E11" s="1">
+        <v>246.22</v>
+      </c>
+      <c r="F11" s="1">
+        <v>208</v>
+      </c>
+      <c r="G11" s="1">
+        <v>172.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2">
-        <v>207</v>
-      </c>
-      <c r="E11" s="2">
-        <v>579.24</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="1">
+        <v>233</v>
+      </c>
+      <c r="C12" s="1">
+        <v>19.22</v>
+      </c>
+      <c r="D12" s="1">
+        <v>255</v>
+      </c>
+      <c r="E12" s="1">
+        <v>53.59</v>
+      </c>
+      <c r="F12" s="1">
+        <v>258</v>
+      </c>
+      <c r="G12" s="1">
+        <v>46.37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2">
-        <v>253</v>
-      </c>
-      <c r="E12" s="2">
-        <v>189.48</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="1">
+        <v>356</v>
+      </c>
+      <c r="C13" s="1">
+        <v>118.91</v>
+      </c>
+      <c r="D13" s="1">
+        <v>377</v>
+      </c>
+      <c r="E13" s="1">
+        <v>499.59</v>
+      </c>
+      <c r="F13" s="1">
+        <v>379</v>
+      </c>
+      <c r="G13" s="1">
+        <v>401.46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2">
-        <v>375</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1213.33</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="1">
+        <v>143</v>
+      </c>
+      <c r="C14" s="1">
+        <v>9.18</v>
+      </c>
+      <c r="D14" s="1">
+        <v>152</v>
+      </c>
+      <c r="E14" s="1">
+        <v>19.05</v>
+      </c>
+      <c r="F14" s="1">
+        <v>154</v>
+      </c>
+      <c r="G14" s="1">
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2">
-        <v>153</v>
-      </c>
-      <c r="E14" s="2">
-        <v>53.25</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2">
-        <v>230</v>
-      </c>
-      <c r="E15" s="2">
-        <v>320.83999999999997</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="B15" s="1">
+        <v>208</v>
+      </c>
+      <c r="C15" s="1">
+        <v>60.8</v>
+      </c>
+      <c r="D15" s="1">
+        <v>232</v>
+      </c>
+      <c r="E15" s="1">
+        <v>241.57</v>
+      </c>
+      <c r="F15" s="1">
+        <v>241</v>
+      </c>
+      <c r="G15" s="1">
+        <v>199.12</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>